<commit_message>
refactor: moved out shared function in tests
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -5,8 +5,8 @@
   <sheets>
     <sheet state="visible" name="Metadata" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Properties" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Container" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="View" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Containers" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Views" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>

</xml_diff>

<commit_message>
refactor; pull out types
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10C11B4-6CDF-44E8-A00D-1A2F27A889C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024573DD-24F8-4888-9F44-819C21814CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="72">
   <si>
     <t>role</t>
   </si>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +332,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -396,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -462,6 +469,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,25 +699,25 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="21" width="11.140625" customWidth="1"/>
-    <col min="22" max="26" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="15" width="11.33203125" customWidth="1"/>
+    <col min="16" max="21" width="11.109375" customWidth="1"/>
+    <col min="22" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8573,25 +8589,25 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="8" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="8" width="13.109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="29" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" customWidth="1"/>
+    <col min="19" max="29" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
@@ -8664,7 +8680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="14.4">
       <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
@@ -8708,7 +8724,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="14.4">
       <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
@@ -8749,7 +8765,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="14.4">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
@@ -8787,7 +8803,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="14.4">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -8825,7 +8841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" ht="14.4">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
@@ -8863,7 +8879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="14.4">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="14"/>
@@ -8875,7 +8891,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="14.4">
       <c r="A9" s="18" t="s">
         <v>50</v>
       </c>
@@ -8913,7 +8929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="14.4">
       <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
@@ -8951,7 +8967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="14.4">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="14"/>
@@ -8963,7 +8979,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="14.4">
       <c r="A12" s="18" t="s">
         <v>53</v>
       </c>
@@ -9001,7 +9017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="18" t="s">
         <v>53</v>
       </c>
@@ -9039,7 +9055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" ht="14.4">
       <c r="A14" s="18" t="s">
         <v>53</v>
       </c>
@@ -9077,7 +9093,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" ht="14.4">
       <c r="A15" s="18" t="s">
         <v>53</v>
       </c>
@@ -9115,7 +9131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" ht="14.4">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="14"/>
@@ -9127,7 +9143,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="14.4">
       <c r="A17" s="18" t="s">
         <v>56</v>
       </c>
@@ -9165,7 +9181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" ht="14.4">
       <c r="A18" s="18" t="s">
         <v>56</v>
       </c>
@@ -9203,7 +9219,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" ht="14.4">
       <c r="A19" s="18" t="s">
         <v>56</v>
       </c>
@@ -9233,7 +9249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" ht="14.4">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="14"/>
@@ -17411,29 +17427,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1002"/>
+  <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="23" width="8.85546875" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="37.5" customHeight="1">
+    <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -17453,84 +17469,105 @@
       <c r="U1" s="21"/>
       <c r="V1" s="21"/>
       <c r="W1" s="21"/>
-    </row>
-    <row r="2" spans="1:23" ht="17.25" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="X1" s="21"/>
+    </row>
+    <row r="2" spans="1:24" ht="17.25" customHeight="1">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:23" ht="33.75" customHeight="1">
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:24" ht="33.75" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:23" ht="33.75" customHeight="1">
+      <c r="B3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:24" ht="33.75" customHeight="1">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="33.75" customHeight="1">
+    <row r="5" spans="1:24" ht="33.75" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="51" customHeight="1">
+    <row r="6" spans="1:24" ht="51" customHeight="1">
       <c r="A6" s="9"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:23" ht="49.5" customHeight="1">
+      <c r="B6" s="9"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:24" ht="49.5" customHeight="1">
       <c r="A7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:23" ht="17.25" customHeight="1">
+      <c r="B7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" ht="17.25" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" ht="17.25" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -18513,10 +18550,10 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18525,29 +18562,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="23" width="8.85546875" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="37.5" customHeight="1">
+    <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -18567,75 +18604,94 @@
       <c r="U1" s="21"/>
       <c r="V1" s="21"/>
       <c r="W1" s="21"/>
-    </row>
-    <row r="2" spans="1:23" ht="17.25" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="X1" s="21"/>
+    </row>
+    <row r="2" spans="1:24" ht="17.25" customHeight="1">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:23" ht="33.75" customHeight="1">
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:24" ht="33.75" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:23" ht="51" customHeight="1">
+      <c r="B3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:24" ht="51" customHeight="1">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="49.5" customHeight="1">
+    <row r="5" spans="1:24" ht="49.5" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17.25" customHeight="1">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:23" ht="17.25" customHeight="1">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -19618,7 +19674,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
refactor add schema to metadata
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024573DD-24F8-4888-9F44-819C21814CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC9BB89-AAE4-4E37-84F4-B8BBD3DC3DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="74">
   <si>
     <t>role</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Implements</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -462,6 +468,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,9 +484,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -725,55 +731,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:23" ht="14.4">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="17.25" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
@@ -785,10 +770,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -814,10 +799,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -843,10 +828,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -872,10 +857,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -901,10 +886,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -930,7 +915,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -958,8 +943,12 @@
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -6233,7 +6222,29 @@
       <c r="W220" s="9"/>
     </row>
     <row r="221" spans="1:23" ht="15.75" customHeight="1">
-      <c r="B221" s="2"/>
+      <c r="A221" s="9"/>
+      <c r="B221" s="4"/>
+      <c r="C221" s="9"/>
+      <c r="D221" s="9"/>
+      <c r="E221" s="9"/>
+      <c r="F221" s="9"/>
+      <c r="G221" s="9"/>
+      <c r="H221" s="9"/>
+      <c r="I221" s="9"/>
+      <c r="J221" s="9"/>
+      <c r="K221" s="9"/>
+      <c r="L221" s="9"/>
+      <c r="M221" s="9"/>
+      <c r="N221" s="9"/>
+      <c r="O221" s="9"/>
+      <c r="P221" s="9"/>
+      <c r="Q221" s="9"/>
+      <c r="R221" s="9"/>
+      <c r="S221" s="9"/>
+      <c r="T221" s="9"/>
+      <c r="U221" s="9"/>
+      <c r="V221" s="9"/>
+      <c r="W221" s="9"/>
     </row>
     <row r="222" spans="1:23" ht="15.75" customHeight="1">
       <c r="B222" s="2"/>
@@ -8571,6 +8582,9 @@
     </row>
     <row r="1000" spans="2:2" ht="15.75" customHeight="1">
       <c r="B1000" s="2"/>
+    </row>
+    <row r="1001" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1001" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -8611,18 +8625,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="10" t="s">
@@ -17430,7 +17444,7 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D5" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -17444,12 +17458,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -17472,7 +17486,7 @@
       <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -18564,8 +18578,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -18579,12 +18593,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -18607,7 +18621,7 @@
       <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="10" t="s">

</xml_diff>

<commit_message>
refactor: working on addid entities
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC9BB89-AAE4-4E37-84F4-B8BBD3DC3DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6491CCC6-177A-4746-99D2-6A3EC9343177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="75">
   <si>
     <t>role</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>circuitBreaker</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,7 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -8599,8 +8602,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -9522,7 +9525,7 @@
         <v>61</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">

</xml_diff>

<commit_message>
[Neat-23] DMS Rules round 2 (#268)
* refactor add schema to metadata

* tests; updated tests

* refactor: add extended

* refactor: working on addid entities

* fix: introduced bug

* refactor; support entity in container and views

* refactor; docs
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024573DD-24F8-4888-9F44-819C21814CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6491CCC6-177A-4746-99D2-6A3EC9343177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="75">
   <si>
     <t>role</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>Implements</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>circuitBreaker</t>
   </si>
 </sst>
 </file>
@@ -462,6 +471,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,9 +487,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,10 +706,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -725,55 +734,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:23" ht="14.4">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="17.25" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
@@ -785,10 +773,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -814,10 +802,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -843,10 +831,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -872,10 +860,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -901,10 +889,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -930,7 +918,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -958,8 +946,12 @@
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -6233,7 +6225,29 @@
       <c r="W220" s="9"/>
     </row>
     <row r="221" spans="1:23" ht="15.75" customHeight="1">
-      <c r="B221" s="2"/>
+      <c r="A221" s="9"/>
+      <c r="B221" s="4"/>
+      <c r="C221" s="9"/>
+      <c r="D221" s="9"/>
+      <c r="E221" s="9"/>
+      <c r="F221" s="9"/>
+      <c r="G221" s="9"/>
+      <c r="H221" s="9"/>
+      <c r="I221" s="9"/>
+      <c r="J221" s="9"/>
+      <c r="K221" s="9"/>
+      <c r="L221" s="9"/>
+      <c r="M221" s="9"/>
+      <c r="N221" s="9"/>
+      <c r="O221" s="9"/>
+      <c r="P221" s="9"/>
+      <c r="Q221" s="9"/>
+      <c r="R221" s="9"/>
+      <c r="S221" s="9"/>
+      <c r="T221" s="9"/>
+      <c r="U221" s="9"/>
+      <c r="V221" s="9"/>
+      <c r="W221" s="9"/>
     </row>
     <row r="222" spans="1:23" ht="15.75" customHeight="1">
       <c r="B222" s="2"/>
@@ -8571,6 +8585,9 @@
     </row>
     <row r="1000" spans="2:2" ht="15.75" customHeight="1">
       <c r="B1000" s="2"/>
+    </row>
+    <row r="1001" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1001" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -8585,8 +8602,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -8611,18 +8628,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="10" t="s">
@@ -9508,7 +9525,7 @@
         <v>61</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">
@@ -17430,7 +17447,7 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D5" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -17444,12 +17461,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -17472,7 +17489,7 @@
       <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -18564,8 +18581,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -18579,12 +18596,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -18607,7 +18624,7 @@
       <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="10" t="s">

</xml_diff>

<commit_message>
refactor; addind missing views and containers to alice
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E020B8-0919-4B05-A43E-3C7B23A8EDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44025147-F078-453E-BE95-9056549F2C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="72">
   <si>
     <t>role</t>
   </si>
@@ -189,9 +189,6 @@
     <t>timeseries</t>
   </si>
   <si>
-    <t>Circuit Breaker</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
   </si>
   <si>
     <t>direct</t>
-  </si>
-  <si>
-    <t>Transmission Line</t>
   </si>
   <si>
     <t>voltageLevel</t>
@@ -733,10 +727,10 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1">
@@ -8599,8 +8593,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8995,7 +8989,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>37</v>
@@ -9025,7 +9019,7 @@
         <v>37</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P12" s="17" t="s">
         <v>37</v>
@@ -9033,7 +9027,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>43</v>
@@ -9063,7 +9057,7 @@
         <v>43</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P13" s="17" t="s">
         <v>43</v>
@@ -9071,10 +9065,10 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="18" t="s">
@@ -9095,21 +9089,21 @@
       </c>
       <c r="J14" s="16"/>
       <c r="M14" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N14" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="P14" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="P14" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>51</v>
@@ -9133,13 +9127,13 @@
       </c>
       <c r="J15" s="16"/>
       <c r="M15" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N15" s="17" t="s">
         <v>51</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P15" s="17" t="s">
         <v>51</v>
@@ -9159,7 +9153,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>37</v>
@@ -9189,7 +9183,7 @@
         <v>37</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>37</v>
@@ -9197,7 +9191,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>41</v>
@@ -9227,7 +9221,7 @@
         <v>43</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P18" s="17" t="s">
         <v>41</v>
@@ -9235,17 +9229,17 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -9253,14 +9247,14 @@
         <v>0</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J19" s="16"/>
       <c r="O19" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -9365,7 +9359,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>37</v>
@@ -9395,7 +9389,7 @@
         <v>37</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>37</v>
@@ -9403,7 +9397,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>41</v>
@@ -9433,7 +9427,7 @@
         <v>41</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P25" s="17" t="s">
         <v>41</v>
@@ -9441,7 +9435,7 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>51</v>
@@ -9465,13 +9459,13 @@
       </c>
       <c r="J26" s="16"/>
       <c r="M26" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N26" s="18" t="s">
         <v>51</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P26" s="17" t="s">
         <v>51</v>
@@ -9479,17 +9473,17 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>62</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="18" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" s="15" t="b">
         <v>1</v>
@@ -9505,31 +9499,31 @@
       </c>
       <c r="J27" s="16"/>
       <c r="M27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N27" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="O27" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="P27" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="15" t="b">
         <v>1</v>
@@ -9545,16 +9539,16 @@
       </c>
       <c r="J28" s="16"/>
       <c r="M28" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1">
@@ -9571,10 +9565,10 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="18" t="s">
@@ -9595,24 +9589,24 @@
       </c>
       <c r="J30" s="16"/>
       <c r="M30" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O30" s="17" t="s">
         <v>64</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="18" t="s">
@@ -9633,24 +9627,24 @@
       </c>
       <c r="J31" s="16"/>
       <c r="M31" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O31" s="17" t="s">
         <v>64</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="18" t="s">
@@ -9671,16 +9665,16 @@
       </c>
       <c r="J32" s="16"/>
       <c r="M32" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="N32" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="O32" s="17" t="s">
         <v>64</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="3:13" ht="15.75" customHeight="1">
@@ -17445,7 +17439,7 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A3:A6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -17460,7 +17454,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -17539,10 +17533,10 @@
     </row>
     <row r="6" spans="1:24" ht="51" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="9" t="s">
@@ -17551,10 +17545,10 @@
     </row>
     <row r="7" spans="1:24" ht="49.5" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -17562,10 +17556,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -18603,8 +18597,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -18619,7 +18613,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="26"/>
@@ -18656,7 +18650,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -18698,10 +18692,10 @@
     </row>
     <row r="6" spans="1:24" ht="17.25" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="9" t="s">
@@ -18710,10 +18704,10 @@
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -18721,10 +18715,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -18744,10 +18738,16 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="9"/>

</xml_diff>

<commit_message>
refactor: support uniqueness constraints
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CF2C79-302B-4B06-8889-72249AE37352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507CA2F-31E5-4430-8118-15F6589FE407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="69">
   <si>
     <t>role</t>
   </si>
@@ -150,13 +150,7 @@
     <t>PowerAsset</t>
   </si>
   <si>
-    <t>unique</t>
-  </si>
-  <si>
     <t>location</t>
-  </si>
-  <si>
-    <t>locaton</t>
   </si>
   <si>
     <t>manufacturer</t>
@@ -724,10 +718,10 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1">
@@ -8591,7 +8585,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="R3" sqref="A3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8726,7 +8720,7 @@
         <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -8734,7 +8728,7 @@
         <v>36</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="13" t="s">
@@ -8758,16 +8752,16 @@
         <v>39</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -8775,7 +8769,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="13" t="s">
@@ -8799,13 +8793,13 @@
         <v>39</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -8813,11 +8807,11 @@
         <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="15" t="b">
@@ -8834,16 +8828,16 @@
       </c>
       <c r="J6" s="16"/>
       <c r="M6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -8851,11 +8845,11 @@
         <v>36</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="15" t="b">
@@ -8875,13 +8869,13 @@
         <v>36</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -8898,7 +8892,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>37</v>
@@ -8928,7 +8922,7 @@
         <v>37</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>37</v>
@@ -8936,14 +8930,14 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="15" t="b">
@@ -8960,16 +8954,16 @@
       </c>
       <c r="J10" s="16"/>
       <c r="M10" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -8986,7 +8980,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>37</v>
@@ -9016,7 +9010,7 @@
         <v>37</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P12" s="17" t="s">
         <v>37</v>
@@ -9024,10 +9018,10 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="18" t="s">
@@ -9051,25 +9045,25 @@
         <v>39</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="15" t="b">
@@ -9086,28 +9080,28 @@
       </c>
       <c r="J14" s="16"/>
       <c r="M14" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="15" t="b">
@@ -9124,16 +9118,16 @@
       </c>
       <c r="J15" s="16"/>
       <c r="M15" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -9150,7 +9144,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>37</v>
@@ -9180,7 +9174,7 @@
         <v>37</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>37</v>
@@ -9188,10 +9182,10 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="18" t="s">
@@ -9215,28 +9209,28 @@
         <v>39</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -9244,14 +9238,14 @@
         <v>0</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J19" s="16"/>
       <c r="O19" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -9268,7 +9262,7 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>37</v>
@@ -9298,7 +9292,7 @@
         <v>37</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P21" s="17" t="s">
         <v>37</v>
@@ -9306,14 +9300,14 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="15" t="b">
@@ -9330,16 +9324,16 @@
       </c>
       <c r="J22" s="16"/>
       <c r="M22" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1">
@@ -9356,7 +9350,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>37</v>
@@ -9386,7 +9380,7 @@
         <v>37</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>37</v>
@@ -9394,10 +9388,10 @@
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="18" t="s">
@@ -9421,25 +9415,25 @@
         <v>39</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="15" t="b">
@@ -9456,31 +9450,31 @@
       </c>
       <c r="J26" s="16"/>
       <c r="M26" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N26" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F27" s="15" t="b">
         <v>1</v>
@@ -9496,31 +9490,31 @@
       </c>
       <c r="J27" s="16"/>
       <c r="M27" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P27" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F28" s="15" t="b">
         <v>1</v>
@@ -9536,16 +9530,16 @@
       </c>
       <c r="J28" s="16"/>
       <c r="M28" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1">
@@ -9562,14 +9556,14 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="15" t="b">
@@ -9586,24 +9580,24 @@
       </c>
       <c r="J30" s="16"/>
       <c r="M30" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="18" t="s">
@@ -9624,24 +9618,24 @@
       </c>
       <c r="J31" s="16"/>
       <c r="M31" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>65</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="18" t="s">
@@ -9662,16 +9656,16 @@
       </c>
       <c r="J32" s="16"/>
       <c r="M32" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N32" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="N32" s="18" t="s">
-        <v>65</v>
-      </c>
       <c r="O32" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P32" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="P32" s="17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="3:13" ht="15.75" customHeight="1">
@@ -17451,7 +17445,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -17506,10 +17500,10 @@
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="17" t="s">
@@ -17525,15 +17519,15 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="51" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="9" t="s">
@@ -17542,10 +17536,10 @@
     </row>
     <row r="7" spans="1:24" ht="49.5" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -17553,10 +17547,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -17565,10 +17559,10 @@
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
@@ -18610,7 +18604,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="26"/>
@@ -18647,7 +18641,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -18665,10 +18659,10 @@
     </row>
     <row r="4" spans="1:24" ht="51" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="17" t="s">
@@ -18684,15 +18678,15 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17.25" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="9" t="s">
@@ -18701,10 +18695,10 @@
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -18712,10 +18706,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -18724,10 +18718,10 @@
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
@@ -18736,10 +18730,10 @@
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">

</xml_diff>

<commit_message>
refactr: added missing relation to MultiEdgeConnection
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053A72DF-2BF4-43EA-92D9-1274D7DD7DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F47BE2-1E8A-4C26-A287-A52816A5F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="68">
   <si>
     <t>role</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>WindFarm</t>
-  </si>
-  <si>
-    <t>WindTurbines</t>
   </si>
   <si>
     <t>multiedge</t>
@@ -394,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -470,7 +467,6 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +715,10 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1">
@@ -8586,7 +8582,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9236,7 +9232,7 @@
       <c r="P18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q18" s="31" t="s">
+      <c r="Q18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -9245,14 +9241,14 @@
         <v>52</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -9260,14 +9256,14 @@
         <v>0</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J19" s="16"/>
       <c r="O19" s="17" t="s">
         <v>52</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -9378,7 +9374,7 @@
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>37</v>
@@ -9408,7 +9404,7 @@
         <v>37</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>37</v>
@@ -9422,7 +9418,7 @@
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>40</v>
@@ -9452,7 +9448,7 @@
         <v>40</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P25" s="17" t="s">
         <v>40</v>
@@ -9463,7 +9459,7 @@
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>48</v>
@@ -9487,13 +9483,13 @@
       </c>
       <c r="J26" s="16"/>
       <c r="M26" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N26" s="18" t="s">
         <v>48</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P26" s="17" t="s">
         <v>48</v>
@@ -9501,17 +9497,17 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>58</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="15" t="b">
         <v>1</v>
@@ -9527,31 +9523,31 @@
       </c>
       <c r="J27" s="16"/>
       <c r="M27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="N27" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="O27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="P27" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F28" s="15" t="b">
         <v>1</v>
@@ -9567,16 +9563,16 @@
       </c>
       <c r="J28" s="16"/>
       <c r="M28" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1">
@@ -9593,10 +9589,10 @@
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="18" t="s">
@@ -9617,24 +9613,24 @@
       </c>
       <c r="J30" s="16"/>
       <c r="M30" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="O30" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="O30" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="P30" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>62</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="18" t="s">
@@ -9655,24 +9651,24 @@
       </c>
       <c r="J31" s="16"/>
       <c r="M31" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N31" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="O31" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="P31" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="P31" s="17" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="18" t="s">
@@ -9693,16 +9689,16 @@
       </c>
       <c r="J32" s="16"/>
       <c r="M32" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="3:13" ht="15.75" customHeight="1">
@@ -17482,7 +17478,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -17573,10 +17569,10 @@
     </row>
     <row r="7" spans="1:24" ht="49.5" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -17584,10 +17580,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -18641,7 +18637,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="26"/>
@@ -18678,7 +18674,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -18732,10 +18728,10 @@
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -18743,10 +18739,10 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">

</xml_diff>

<commit_message>
[NEAT-25] Rules <-> DMS (#271)
* refactor add schema to metadata

* tests; updated tests

* refactor: add extended

* refactor: working on addid entities

* fix: introduced bug

* refactor; support entity in container and views

* refactor; docs

* refactor: moved out to DMS exporter

* tests; fix data

* refactor; setup shell for importer

* refactor: first pass on DMS improter

* refactor: working on matching

* refactor: ignore extra fields

* refactor: added missing version

* refactor: upgrade

* refactor; addind missing views and containers to alice

* refactor; addind missing views and containers to alice

* refactor: implemented require constraint

* refactor: handle direct relatinos

* refactor: support uniqueness constraints

* refactor: unique constraint

* refactor: index implemented

* refactr: added missing relation to MultiEdgeConnection

* refactor: fix tests
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6491CCC6-177A-4746-99D2-6A3EC9343177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F47BE2-1E8A-4C26-A287-A52816A5F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="68">
   <si>
     <t>role</t>
   </si>
@@ -150,13 +150,7 @@
     <t>PowerAsset</t>
   </si>
   <si>
-    <t>unique</t>
-  </si>
-  <si>
     <t>location</t>
-  </si>
-  <si>
-    <t>locaton</t>
   </si>
   <si>
     <t>manufacturer</t>
@@ -174,9 +168,6 @@
     <t>activePower</t>
   </si>
   <si>
-    <t>ratedPowe</t>
-  </si>
-  <si>
     <t>hubHeight</t>
   </si>
   <si>
@@ -189,9 +180,6 @@
     <t>timeseries</t>
   </si>
   <si>
-    <t>Circuit Breaker</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -199,9 +187,6 @@
   </si>
   <si>
     <t>WindFarm</t>
-  </si>
-  <si>
-    <t>WindTurbines</t>
   </si>
   <si>
     <t>multiedge</t>
@@ -220,12 +205,6 @@
   </si>
   <si>
     <t>direct</t>
-  </si>
-  <si>
-    <t>circuit breaker</t>
-  </si>
-  <si>
-    <t>Transmission Line</t>
   </si>
   <si>
     <t>voltageLevel</t>
@@ -712,21 +691,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" customWidth="1"/>
-    <col min="6" max="6" width="51.109375" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="15" width="11.33203125" customWidth="1"/>
-    <col min="16" max="21" width="11.109375" customWidth="1"/>
-    <col min="22" max="26" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" customWidth="1"/>
+    <col min="6" max="6" width="51.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="21" width="11.140625" customWidth="1"/>
+    <col min="22" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.4">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,12 +713,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="14.4">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1">
@@ -8603,28 +8582,28 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="8" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
-    <col min="14" max="14" width="24.5546875" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" customWidth="1"/>
-    <col min="16" max="16" width="18.5546875" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" customWidth="1"/>
-    <col min="19" max="29" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="29" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
@@ -8697,7 +8676,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4">
+    <row r="3" spans="1:18">
       <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
@@ -8738,15 +8717,15 @@
         <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="14.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="13" t="s">
@@ -8770,24 +8749,24 @@
         <v>39</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="14.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="13" t="s">
@@ -8811,25 +8790,25 @@
         <v>39</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="14.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="15" t="b">
@@ -8846,28 +8825,28 @@
       </c>
       <c r="J6" s="16"/>
       <c r="M6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="14.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="15" t="b">
@@ -8887,16 +8866,16 @@
         <v>36</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>36</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="14.4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="14"/>
@@ -8908,9 +8887,9 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:18" ht="14.4">
+    <row r="9" spans="1:18">
       <c r="A9" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>37</v>
@@ -8940,22 +8919,28 @@
         <v>37</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="14.4">
+      <c r="Q9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="15" t="b">
@@ -8972,19 +8957,19 @@
       </c>
       <c r="J10" s="16"/>
       <c r="M10" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="14.4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="14"/>
@@ -8996,9 +8981,9 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:18" ht="14.4">
+    <row r="12" spans="1:18">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>37</v>
@@ -9028,18 +9013,24 @@
         <v>37</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P12" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="14.4">
+      <c r="Q12" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="18" t="s">
@@ -9063,25 +9054,25 @@
         <v>39</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="14.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="15" t="b">
@@ -9098,28 +9089,28 @@
       </c>
       <c r="J14" s="16"/>
       <c r="M14" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="14.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="15" t="b">
@@ -9136,19 +9127,19 @@
       </c>
       <c r="J15" s="16"/>
       <c r="M15" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O15" s="17" t="s">
-        <v>53</v>
-      </c>
       <c r="P15" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="14.4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="14"/>
@@ -9160,9 +9151,9 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:16" ht="14.4">
+    <row r="17" spans="1:18">
       <c r="A17" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>37</v>
@@ -9192,18 +9183,24 @@
         <v>37</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="14.4">
+      <c r="Q17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="18" t="s">
@@ -9227,28 +9224,31 @@
         <v>39</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14.4">
+        <v>40</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -9256,17 +9256,17 @@
         <v>0</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J19" s="16"/>
       <c r="O19" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="14"/>
@@ -9278,9 +9278,9 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>37</v>
@@ -9310,22 +9310,28 @@
         <v>37</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P21" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1">
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="15" t="b">
@@ -9342,19 +9348,19 @@
       </c>
       <c r="J22" s="16"/>
       <c r="M22" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="14"/>
@@ -9366,9 +9372,9 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>37</v>
@@ -9398,18 +9404,24 @@
         <v>37</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1">
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="18" t="s">
@@ -9433,25 +9445,28 @@
         <v>39</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1">
+        <v>40</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="15" t="b">
@@ -9468,31 +9483,31 @@
       </c>
       <c r="J26" s="16"/>
       <c r="M26" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N26" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F27" s="15" t="b">
         <v>1</v>
@@ -9508,31 +9523,31 @@
       </c>
       <c r="J27" s="16"/>
       <c r="M27" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P27" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F28" s="15" t="b">
         <v>1</v>
@@ -9548,19 +9563,19 @@
       </c>
       <c r="J28" s="16"/>
       <c r="M28" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="14"/>
@@ -9572,16 +9587,16 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="15" t="b">
@@ -9598,24 +9613,24 @@
       </c>
       <c r="J30" s="16"/>
       <c r="M30" s="17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="18" t="s">
@@ -9636,24 +9651,24 @@
       </c>
       <c r="J31" s="16"/>
       <c r="M31" s="17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="18" t="s">
@@ -9674,27 +9689,28 @@
       </c>
       <c r="J32" s="16"/>
       <c r="M32" s="17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="15.75" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" ht="15.75" customHeight="1">
       <c r="C33" s="20"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="3:10" ht="15.75" customHeight="1">
+      <c r="M33" s="17"/>
+    </row>
+    <row r="34" spans="3:13" ht="15.75" customHeight="1">
       <c r="C34" s="20"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -9702,7 +9718,7 @@
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
     </row>
-    <row r="35" spans="3:10" ht="15.75" customHeight="1">
+    <row r="35" spans="3:13" ht="15.75" customHeight="1">
       <c r="C35" s="20"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -9710,7 +9726,7 @@
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
     </row>
-    <row r="36" spans="3:10" ht="15.75" customHeight="1">
+    <row r="36" spans="3:13" ht="15.75" customHeight="1">
       <c r="C36" s="20"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -9718,7 +9734,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
     </row>
-    <row r="37" spans="3:10" ht="15.75" customHeight="1">
+    <row r="37" spans="3:13" ht="15.75" customHeight="1">
       <c r="C37" s="20"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -9726,7 +9742,7 @@
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
     </row>
-    <row r="38" spans="3:10" ht="15.75" customHeight="1">
+    <row r="38" spans="3:13" ht="15.75" customHeight="1">
       <c r="C38" s="20"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -9734,7 +9750,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
     </row>
-    <row r="39" spans="3:10" ht="15.75" customHeight="1">
+    <row r="39" spans="3:13" ht="15.75" customHeight="1">
       <c r="C39" s="20"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -9742,7 +9758,7 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
     </row>
-    <row r="40" spans="3:10" ht="15.75" customHeight="1">
+    <row r="40" spans="3:13" ht="15.75" customHeight="1">
       <c r="C40" s="20"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -9750,7 +9766,7 @@
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
     </row>
-    <row r="41" spans="3:10" ht="15.75" customHeight="1">
+    <row r="41" spans="3:13" ht="15.75" customHeight="1">
       <c r="C41" s="20"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -9758,7 +9774,7 @@
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
     </row>
-    <row r="42" spans="3:10" ht="15.75" customHeight="1">
+    <row r="42" spans="3:13" ht="15.75" customHeight="1">
       <c r="C42" s="20"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -9766,7 +9782,7 @@
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
     </row>
-    <row r="43" spans="3:10" ht="15.75" customHeight="1">
+    <row r="43" spans="3:13" ht="15.75" customHeight="1">
       <c r="C43" s="20"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
@@ -9774,7 +9790,7 @@
       <c r="I43" s="16"/>
       <c r="J43" s="16"/>
     </row>
-    <row r="44" spans="3:10" ht="15.75" customHeight="1">
+    <row r="44" spans="3:13" ht="15.75" customHeight="1">
       <c r="C44" s="20"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
@@ -9782,7 +9798,7 @@
       <c r="I44" s="16"/>
       <c r="J44" s="16"/>
     </row>
-    <row r="45" spans="3:10" ht="15.75" customHeight="1">
+    <row r="45" spans="3:13" ht="15.75" customHeight="1">
       <c r="C45" s="20"/>
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
@@ -9790,7 +9806,7 @@
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
     </row>
-    <row r="46" spans="3:10" ht="15.75" customHeight="1">
+    <row r="46" spans="3:13" ht="15.75" customHeight="1">
       <c r="C46" s="20"/>
       <c r="F46" s="16"/>
       <c r="G46" s="16"/>
@@ -9798,7 +9814,7 @@
       <c r="I46" s="16"/>
       <c r="J46" s="16"/>
     </row>
-    <row r="47" spans="3:10" ht="15.75" customHeight="1">
+    <row r="47" spans="3:13" ht="15.75" customHeight="1">
       <c r="C47" s="20"/>
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
@@ -9806,7 +9822,7 @@
       <c r="I47" s="16"/>
       <c r="J47" s="16"/>
     </row>
-    <row r="48" spans="3:10" ht="15.75" customHeight="1">
+    <row r="48" spans="3:13" ht="15.75" customHeight="1">
       <c r="C48" s="20"/>
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
@@ -17447,22 +17463,22 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A3:D5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="24" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="24" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -17517,10 +17533,10 @@
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="17" t="s">
@@ -17536,31 +17552,55 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="51" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:24" ht="49.5" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="9"/>
@@ -18582,22 +18622,22 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D5"/>
+      <selection activeCell="D11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="24" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="24" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="26"/>
@@ -18634,7 +18674,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -18652,10 +18692,10 @@
     </row>
     <row r="4" spans="1:24" ht="51" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="17" t="s">
@@ -18671,38 +18711,67 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="9"/>

</xml_diff>

<commit_message>
tests: added failing test in validation
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F47BE2-1E8A-4C26-A287-A52816A5F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992FF68-DFE3-4F83-8CAA-95934FB72750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
   <si>
     <t>role</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>circuitBreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -691,21 +694,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="21" width="11.140625" customWidth="1"/>
-    <col min="22" max="26" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="15" width="11.33203125" customWidth="1"/>
+    <col min="16" max="21" width="11.109375" customWidth="1"/>
+    <col min="22" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="14.4">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -8582,28 +8585,28 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="8" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="8" width="13.109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="29" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" customWidth="1"/>
+    <col min="19" max="29" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
@@ -8676,7 +8679,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="14.4">
       <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
@@ -8720,7 +8723,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="14.4">
       <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="14.4">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
@@ -8799,7 +8802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="14.4">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -8836,8 +8839,11 @@
       <c r="P6" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="14.4">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
@@ -8875,7 +8881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="14.4">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="14"/>
@@ -8887,7 +8893,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="14.4">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -8924,14 +8930,8 @@
       <c r="P9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+    </row>
+    <row r="10" spans="1:18" ht="14.4">
       <c r="A10" s="18" t="s">
         <v>47</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="14.4">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="14"/>
@@ -8981,7 +8981,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="14.4">
       <c r="A12" s="18" t="s">
         <v>51</v>
       </c>
@@ -9018,14 +9018,8 @@
       <c r="P12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q12" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+    </row>
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="18" t="s">
         <v>51</v>
       </c>
@@ -9063,7 +9057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" ht="14.4">
       <c r="A14" s="18" t="s">
         <v>51</v>
       </c>
@@ -9101,7 +9095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" ht="14.4">
       <c r="A15" s="18" t="s">
         <v>51</v>
       </c>
@@ -9139,7 +9133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" ht="14.4">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="14"/>
@@ -9151,7 +9145,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:16" ht="14.4">
       <c r="A17" s="18" t="s">
         <v>52</v>
       </c>
@@ -9188,14 +9182,8 @@
       <c r="P17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+    </row>
+    <row r="18" spans="1:16" ht="14.4">
       <c r="A18" s="18" t="s">
         <v>52</v>
       </c>
@@ -9232,11 +9220,8 @@
       <c r="P18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+    </row>
+    <row r="19" spans="1:16" ht="14.4">
       <c r="A19" s="18" t="s">
         <v>52</v>
       </c>
@@ -9266,7 +9251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:16" ht="14.4">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="14"/>
@@ -9278,7 +9263,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>44</v>
       </c>
@@ -9315,14 +9300,8 @@
       <c r="P21" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" t="s">
-        <v>37</v>
-      </c>
-      <c r="R21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
@@ -9360,7 +9339,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="14"/>
@@ -9372,7 +9351,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>56</v>
       </c>
@@ -9409,14 +9388,8 @@
       <c r="P24" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q24" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
@@ -9453,11 +9426,8 @@
       <c r="P25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
         <v>56</v>
       </c>
@@ -9495,7 +9465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
         <v>56</v>
       </c>
@@ -9535,7 +9505,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -9575,7 +9545,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="14"/>
@@ -9587,7 +9557,7 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
         <v>60</v>
       </c>
@@ -9625,7 +9595,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
         <v>60</v>
       </c>
@@ -9663,7 +9633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
         <v>60</v>
       </c>
@@ -17463,17 +17433,17 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E15" sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="24" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
@@ -18622,17 +18592,17 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="24" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">

</xml_diff>

<commit_message>
[NEAT-27] DMS sheet validation (#273)
* refactor; extend dms rules to lists

* refactor: Fix issues with mulit-constraints

* fix: None for empty constraints

* tests: added failing test case for direct and multiedge connection

* refactor; Handle parsing on relations correctly

* refactor: Correct serialization

* tests: added failing test in validation

* feat: Implemented validation of property sheet
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\tutorial\use-cases\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F47BE2-1E8A-4C26-A287-A52816A5F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992FF68-DFE3-4F83-8CAA-95934FB72750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
   <si>
     <t>role</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>circuitBreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -691,21 +694,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="21" width="11.140625" customWidth="1"/>
-    <col min="22" max="26" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="15" width="11.33203125" customWidth="1"/>
+    <col min="16" max="21" width="11.109375" customWidth="1"/>
+    <col min="22" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="14.4">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -8582,28 +8585,28 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="8" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="8" width="13.109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="29" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" customWidth="1"/>
+    <col min="19" max="29" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1">
@@ -8676,7 +8679,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="14.4">
       <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
@@ -8720,7 +8723,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="14.4">
       <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="14.4">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
@@ -8799,7 +8802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="14.4">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -8836,8 +8839,11 @@
       <c r="P6" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="14.4">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
@@ -8875,7 +8881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="14.4">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="14"/>
@@ -8887,7 +8893,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="14.4">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -8924,14 +8930,8 @@
       <c r="P9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+    </row>
+    <row r="10" spans="1:18" ht="14.4">
       <c r="A10" s="18" t="s">
         <v>47</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="14.4">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="14"/>
@@ -8981,7 +8981,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="14.4">
       <c r="A12" s="18" t="s">
         <v>51</v>
       </c>
@@ -9018,14 +9018,8 @@
       <c r="P12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q12" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+    </row>
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="18" t="s">
         <v>51</v>
       </c>
@@ -9063,7 +9057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" ht="14.4">
       <c r="A14" s="18" t="s">
         <v>51</v>
       </c>
@@ -9101,7 +9095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" ht="14.4">
       <c r="A15" s="18" t="s">
         <v>51</v>
       </c>
@@ -9139,7 +9133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" ht="14.4">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="14"/>
@@ -9151,7 +9145,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:16" ht="14.4">
       <c r="A17" s="18" t="s">
         <v>52</v>
       </c>
@@ -9188,14 +9182,8 @@
       <c r="P17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+    </row>
+    <row r="18" spans="1:16" ht="14.4">
       <c r="A18" s="18" t="s">
         <v>52</v>
       </c>
@@ -9232,11 +9220,8 @@
       <c r="P18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+    </row>
+    <row r="19" spans="1:16" ht="14.4">
       <c r="A19" s="18" t="s">
         <v>52</v>
       </c>
@@ -9266,7 +9251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:16" ht="14.4">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="14"/>
@@ -9278,7 +9263,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>44</v>
       </c>
@@ -9315,14 +9300,8 @@
       <c r="P21" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" t="s">
-        <v>37</v>
-      </c>
-      <c r="R21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
@@ -9360,7 +9339,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="14"/>
@@ -9372,7 +9351,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>56</v>
       </c>
@@ -9409,14 +9388,8 @@
       <c r="P24" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q24" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
@@ -9453,11 +9426,8 @@
       <c r="P25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
         <v>56</v>
       </c>
@@ -9495,7 +9465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
         <v>56</v>
       </c>
@@ -9535,7 +9505,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -9575,7 +9545,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="14"/>
@@ -9587,7 +9557,7 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="18" t="s">
         <v>60</v>
       </c>
@@ -9625,7 +9595,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
         <v>60</v>
       </c>
@@ -9663,7 +9633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
         <v>60</v>
       </c>
@@ -17463,17 +17433,17 @@
   <dimension ref="A1:X1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E15" sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="24" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">
@@ -18622,17 +18592,17 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="24" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1">

</xml_diff>

<commit_message>
reorg of code base
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/tutorial/use-cases/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF8EF27-FE8B-FC4F-AB2A-0D03B3CE5A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB734E26-3DF9-CD46-88C7-BEEB7D977D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17600" yWindow="4400" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
-    <sheet name="Containers" sheetId="3" r:id="rId3"/>
-    <sheet name="Views" sheetId="4" r:id="rId4"/>
+    <sheet name="Views" sheetId="4" r:id="rId2"/>
+    <sheet name="Properties" sheetId="2" r:id="rId3"/>
+    <sheet name="Containers" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -253,53 +253,63 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -310,18 +320,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -469,6 +482,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -482,15 +504,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,8 +725,8 @@
   </sheetPr>
   <dimension ref="A1:W1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -863,10 +876,10 @@
       <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="9"/>
@@ -921,7 +934,7 @@
       <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="25" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -950,10 +963,10 @@
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="27">
         <v>45331</v>
       </c>
       <c r="C10" s="9"/>
@@ -979,10 +992,10 @@
       <c r="W10" s="9"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="27">
         <v>45331</v>
       </c>
       <c r="C11" s="9"/>
@@ -8629,14 +8642,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:X1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="24" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+    </row>
+    <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8661,18 +9827,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -17476,7 +18642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -17498,12 +18664,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -18633,1157 +19799,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:X1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
-    <col min="7" max="24" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-    </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>